<commit_message>
Update DateBase/orders/Fresh bloom Flowers_2025-10-7.xlsx
</commit_message>
<xml_diff>
--- a/DateBase/orders/Fresh bloom Flowers_2025-10-7.xlsx
+++ b/DateBase/orders/Fresh bloom Flowers_2025-10-7.xlsx
@@ -874,6 +874,9 @@
       <c r="C51" t="str">
         <v>577_腊梅白_wax white_undefined_1bunch</v>
       </c>
+      <c r="F51" t="str">
+        <v>2</v>
+      </c>
     </row>
   </sheetData>
   <ignoredErrors>
@@ -935,7 +938,7 @@
         <v>0.00</v>
       </c>
       <c r="G2" t="str">
-        <v>013242011.5111253551013822121431751240503325531555211091029323555555554512520100</v>
+        <v>013242011.5111253551013822121431751240503325531555211091029323555555554512520102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>